<commit_message>
set default worksheet to Authors
</commit_message>
<xml_diff>
--- a/docs/assets/files/AuthorArranger Sample.xlsx
+++ b/docs/assets/files/AuthorArranger Sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="56295" yWindow="8940" windowWidth="30960" windowHeight="17625" activeTab="1"/>
+    <workbookView xWindow="56295" yWindow="8940" windowWidth="30960" windowHeight="17625" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Directions" sheetId="1" r:id="rId1"/>
@@ -17264,7 +17264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -17562,7 +17562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>